<commit_message>
Add different palette types
Added new XML for formatting palettes
</commit_message>
<xml_diff>
--- a/formatting colors/format.xlsx
+++ b/formatting colors/format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="9660"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="9660" activeTab="3"/>
   </bookViews>
   <sheets>
     <sheet name="dark" sheetId="1" r:id="rId1"/>
@@ -865,7 +865,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:N36"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
@@ -3472,8 +3472,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M12"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="M21" sqref="M21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="M12" sqref="M12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
new palettes, bug fixes
</commit_message>
<xml_diff>
--- a/formatting colors/format.xlsx
+++ b/formatting colors/format.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="9660" activeTab="3"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="21540" windowHeight="9660" activeTab="2"/>
   </bookViews>
   <sheets>
     <sheet name="dark" sheetId="1" r:id="rId1"/>
@@ -20,7 +20,7 @@
   <definedNames>
     <definedName name="SwatchesPrefsName" localSheetId="0">dark!$A$1:$I$169</definedName>
   </definedNames>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="152511" concurrentCalc="0"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -47,7 +47,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="718" uniqueCount="121">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="152">
   <si>
     <t>&lt;preference</t>
   </si>
@@ -410,6 +410,99 @@
   </si>
   <si>
     <t>&lt;preference key='swatch.dark.eighthcol.firstrow' value='#26794A' /&gt;</t>
+  </si>
+  <si>
+    <t>#1F77B4</t>
+  </si>
+  <si>
+    <t>#FF7F0E</t>
+  </si>
+  <si>
+    <t>#2CA02C</t>
+  </si>
+  <si>
+    <t>#D62728</t>
+  </si>
+  <si>
+    <t>#9467BD</t>
+  </si>
+  <si>
+    <t>#8C564B</t>
+  </si>
+  <si>
+    <t>#E377C2</t>
+  </si>
+  <si>
+    <t>#7F7F7F</t>
+  </si>
+  <si>
+    <t>#BCBD22</t>
+  </si>
+  <si>
+    <t>#17BECF</t>
+  </si>
+  <si>
+    <t>medium</t>
+  </si>
+  <si>
+    <t>#729ECE</t>
+  </si>
+  <si>
+    <t>#FF9E4A</t>
+  </si>
+  <si>
+    <t>#67BF5C</t>
+  </si>
+  <si>
+    <t>#ED665D</t>
+  </si>
+  <si>
+    <t>#AD8BC9</t>
+  </si>
+  <si>
+    <t>#A8786E</t>
+  </si>
+  <si>
+    <t>#ED97CA</t>
+  </si>
+  <si>
+    <t>#A2A2A2</t>
+  </si>
+  <si>
+    <t>#CDCC5D</t>
+  </si>
+  <si>
+    <t>#6DCCDA</t>
+  </si>
+  <si>
+    <t>#AEC7E8</t>
+  </si>
+  <si>
+    <t>#FFBB78</t>
+  </si>
+  <si>
+    <t>#98DF8A</t>
+  </si>
+  <si>
+    <t>#FF9896</t>
+  </si>
+  <si>
+    <t>#C5B0D5</t>
+  </si>
+  <si>
+    <t>#C49C94</t>
+  </si>
+  <si>
+    <t>#F7B6D2</t>
+  </si>
+  <si>
+    <t>#C7C7C7</t>
+  </si>
+  <si>
+    <t>#DBDB8D</t>
+  </si>
+  <si>
+    <t>#9EDAE5</t>
   </si>
 </sst>
 </file>
@@ -2100,7 +2193,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="B1:M42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="M13" sqref="M13"/>
     </sheetView>
   </sheetViews>
@@ -3470,10 +3563,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="B1:M12"/>
+  <dimension ref="B1:O27"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="M12" sqref="M12"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="M18" sqref="M18:O27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -3800,6 +3893,127 @@
         <v>118</v>
       </c>
     </row>
+    <row r="17" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M17" t="s">
+        <v>100</v>
+      </c>
+      <c r="N17" t="s">
+        <v>131</v>
+      </c>
+      <c r="O17" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="18" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M18" t="s">
+        <v>121</v>
+      </c>
+      <c r="N18" t="s">
+        <v>132</v>
+      </c>
+      <c r="O18" t="s">
+        <v>142</v>
+      </c>
+    </row>
+    <row r="19" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M19" t="s">
+        <v>122</v>
+      </c>
+      <c r="N19" t="s">
+        <v>133</v>
+      </c>
+      <c r="O19" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="20" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M20" t="s">
+        <v>123</v>
+      </c>
+      <c r="N20" t="s">
+        <v>134</v>
+      </c>
+      <c r="O20" t="s">
+        <v>144</v>
+      </c>
+    </row>
+    <row r="21" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M21" t="s">
+        <v>124</v>
+      </c>
+      <c r="N21" t="s">
+        <v>135</v>
+      </c>
+      <c r="O21" t="s">
+        <v>145</v>
+      </c>
+    </row>
+    <row r="22" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M22" t="s">
+        <v>125</v>
+      </c>
+      <c r="N22" t="s">
+        <v>136</v>
+      </c>
+      <c r="O22" t="s">
+        <v>146</v>
+      </c>
+    </row>
+    <row r="23" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M23" t="s">
+        <v>126</v>
+      </c>
+      <c r="N23" t="s">
+        <v>137</v>
+      </c>
+      <c r="O23" t="s">
+        <v>147</v>
+      </c>
+    </row>
+    <row r="24" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M24" t="s">
+        <v>127</v>
+      </c>
+      <c r="N24" t="s">
+        <v>138</v>
+      </c>
+      <c r="O24" t="s">
+        <v>148</v>
+      </c>
+    </row>
+    <row r="25" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M25" t="s">
+        <v>128</v>
+      </c>
+      <c r="N25" t="s">
+        <v>139</v>
+      </c>
+      <c r="O25" t="s">
+        <v>149</v>
+      </c>
+    </row>
+    <row r="26" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M26" t="s">
+        <v>129</v>
+      </c>
+      <c r="N26" t="s">
+        <v>140</v>
+      </c>
+      <c r="O26" t="s">
+        <v>150</v>
+      </c>
+    </row>
+    <row r="27" spans="13:15" x14ac:dyDescent="0.25">
+      <c r="M27" t="s">
+        <v>130</v>
+      </c>
+      <c r="N27" t="s">
+        <v>141</v>
+      </c>
+      <c r="O27" t="s">
+        <v>151</v>
+      </c>
+    </row>
   </sheetData>
   <sortState ref="B1:I26">
     <sortCondition ref="D1:D26"/>

</xml_diff>